<commit_message>
add new handler data from timer
</commit_message>
<xml_diff>
--- a/72.xlsx
+++ b/72.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185B1504-651A-429D-AE80-CDECF7AFEE09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -85,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,20 +395,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -441,7 +440,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -459,7 +458,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -467,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -478,7 +477,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -493,7 +492,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -509,7 +508,7 @@
         <v>1150.1597444089457</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -521,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>B1/(B2*B3)</f>
         <v>1150.1597444089457</v>
@@ -537,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>A10/1000</f>
         <v>1.1501597444089458</v>
@@ -553,7 +552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>A11/1000</f>
         <v>1.1501597444089457E-3</v>
@@ -569,7 +568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -583,43 +582,43 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
       </c>
       <c r="G19">
         <f>B18/(G24*B20*B21)</f>
-        <v>2.447148392359459</v>
+        <v>2.3567921440261865</v>
       </c>
       <c r="I19">
         <v>65535</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>62600</v>
+        <v>65000</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
       </c>
       <c r="G20">
         <f>B18/(G24*B19*B21)</f>
-        <v>153191.48936170212</v>
+        <v>2127.6595744680849</v>
       </c>
       <c r="I20">
         <v>65535</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -627,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -638,13 +637,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
       <c r="C24">
         <f>C27*1000000000</f>
-        <v>869444.44444444438</v>
+        <v>65000000</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -653,77 +652,77 @@
         <v>470</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
       <c r="C25">
         <f>C27*1000000</f>
-        <v>869.44444444444434</v>
+        <v>65000</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="G25">
         <f>B18/(B19*B20*B21)</f>
-        <v>1150.1597444089457</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15.384615384615385</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
       <c r="C26">
         <f>C27*1000</f>
-        <v>0.86944444444444435</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>B18/(B19*B20)</f>
-        <v>1150.1597444089457</v>
+        <v>15.384615384615385</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27">
         <f>1/A27</f>
-        <v>8.6944444444444439E-4</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>A27/1000</f>
-        <v>1.1501597444089458</v>
+        <v>1.5384615384615385E-2</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28">
         <f>C27/60</f>
-        <v>1.449074074074074E-5</v>
+        <v>1.0833333333333333E-3</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>A28/1000</f>
-        <v>1.1501597444089457E-3</v>
+        <v>1.5384615384615384E-5</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
       <c r="C29">
         <f>C28/60</f>
-        <v>2.4151234567901235E-7</v>
+        <v>1.8055555555555555E-5</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>

</xml_diff>